<commit_message>
GDD & variables edit
</commit_message>
<xml_diff>
--- a/Variables/Variables.xlsx
+++ b/Variables/Variables.xlsx
@@ -3,31 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C89458-8EE7-4A86-A9EF-368D0F2F850B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C5ED23-A8AF-4E34-BF62-CA0627042AAB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="2" r:id="rId1"/>
     <sheet name="Entities" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="41">
   <si>
     <t>attack speed</t>
   </si>
@@ -65,9 +59,6 @@
     <t>Boss</t>
   </si>
   <si>
-    <t>Entities</t>
-  </si>
-  <si>
     <t>hp</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>Enemy base stats</t>
   </si>
   <si>
-    <t>Kolom1</t>
-  </si>
-  <si>
     <t>Auto archer</t>
   </si>
   <si>
@@ -144,6 +132,18 @@
   </si>
   <si>
     <t>Player base stats</t>
+  </si>
+  <si>
+    <t>Enemy max stats</t>
+  </si>
+  <si>
+    <t>Player max stats</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Multipliers</t>
   </si>
 </sst>
 </file>
@@ -151,9 +151,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,16 +176,70 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -212,21 +266,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -250,7 +289,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -258,6 +297,21 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -269,14 +323,31 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -289,106 +360,182 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+  <cellStyles count="7">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="5" builtinId="23"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="6" builtinId="10"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="40">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -550,10 +697,9 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -590,7 +736,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -630,7 +775,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -670,7 +814,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -709,7 +852,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -748,7 +890,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -787,7 +928,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -826,7 +966,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -865,7 +1004,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -904,7 +1042,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -943,7 +1080,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -981,7 +1117,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -999,7 +1134,608 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1018,25 +1754,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D42D5E63-5628-4C03-A1BA-BCD09666E9A7}" name="Tabel2" displayName="Tabel2" ref="A2:K7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A2:K7" xr:uid="{0C2BE41B-9E37-42D9-A245-D19AC6CC0C81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel2" displayName="Tabel2" ref="A15:K20" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A15:K20" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{3C4DE866-3A29-4195-A063-468C570502E4}" name="Entities" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{9E571F5F-8BDF-4628-BB46-F8CC42EB4630}" name="hp" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{DD8367C8-84C5-4247-B36D-5BAF4CBF33EB}" name="do" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{0B9E2CF4-CC3C-4AD8-9318-25086170C17B}" name="as" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{668AEE06-F6B4-40BD-8B22-B476A7EA01B1}" name="ms" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1728C296-A359-4B32-8457-BB3F1A85A94F}" name="ps" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{36373F1A-8F05-4054-8768-419CBC728D50}" name="ad" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{2017922E-2308-422F-8B42-9B735E0DE28A}" name="cv" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{04C637C5-B79C-410D-B62E-372F687201E3}" name="dps" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Entity" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="hp" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="do" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="as" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ms" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="ps" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ad" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="cv" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="dps" dataDxfId="29">
       <calculatedColumnFormula>PRODUCT(Tabel2[[#This Row],[do]:[as]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{B0C86B91-0D6F-4AB1-9C14-426FAEC442E2}" name="score (hp*ms*dps + ps + ad)" dataDxfId="8">
-      <calculatedColumnFormula>MROUND(PRODUCT(B3,E3,I3), 1) + F3 + G3</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="score (hp*ms*dps + ps + ad)" dataDxfId="28">
+      <calculatedColumnFormula>MROUND(PRODUCT(B16,E16,I16), 1) + F16 + G16</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{003CC407-73EE-42E1-904D-71E147FCB801}" name="cv / score ratio" dataDxfId="7" dataCellStyle="Komma">
-      <calculatedColumnFormula>H3/J3</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="cv / score ratio" dataDxfId="27">
+      <calculatedColumnFormula>H16/J16</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1044,16 +1780,59 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3995C526-4316-4F61-94C8-B3195E3431B4}" name="Tabel1" displayName="Tabel1" ref="A15:F17" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A15:F17" xr:uid="{D08510D1-D8A8-4CB5-8F81-4FD4A6438D4B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabel1" displayName="Tabel1" ref="A28:F30" totalsRowShown="0" headerRowDxfId="26">
+  <autoFilter ref="A28:F30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7344EE0A-A296-4F42-BC0D-899006A1730E}" name="Kolom1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E00FBF54-9F40-4A78-8638-AB6C609FDEB8}" name="hp" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{EEA00FDD-2458-4FDF-A78F-4B52EE847006}" name="do" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{9666B07C-9B35-45E3-B466-BC29EBA11D8D}" name="as" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E0E297A6-762B-4801-B21D-A37966C89E58}" name="ps" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{3CDCA593-118B-4931-B108-442EB7A72317}" name="dps" dataDxfId="0">
-      <calculatedColumnFormula>PRODUCT(C16,D16)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Entity" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="hp" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="do" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="as" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ps" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="dps" dataDxfId="20">
+      <calculatedColumnFormula>PRODUCT(C29,D29)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabel24" displayName="Tabel24" ref="M16:W22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="M16:W22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Entity" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="hp" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="do" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="as" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="ms" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="ps" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="ad" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="cv" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="dps" dataDxfId="9">
+      <calculatedColumnFormula>PRODUCT(Tabel24[[#This Row],[do]:[as]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="score (hp*ms*dps + ps + ad)" dataDxfId="8">
+      <calculatedColumnFormula>MROUND(PRODUCT(N17,Q17,U17), 1) + R17 + S17</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="cv / score ratio" dataDxfId="7">
+      <calculatedColumnFormula>T17/V17</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabel15" displayName="Tabel15" ref="M29:R31" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="M29:R31" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Entity" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="hp" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="do" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="as" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="ps" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="dps" dataDxfId="0">
+      <calculatedColumnFormula>PRODUCT(O30,P30)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1322,101 +2101,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAB738C-ED4C-4F6D-9628-53F6986D4203}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B2" s="37"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>1</v>
+      <c r="B4" s="34" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
+      <c r="B5" s="34" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
+      <c r="B6" s="34" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+      <c r="B7" s="34" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
+      <c r="B8" s="34" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
+      <c r="B9" s="34" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1424,337 +2202,697 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A13:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="8" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" customWidth="1"/>
-    <col min="12" max="18" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="8" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="18" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="28.42578125" customWidth="1"/>
+    <col min="23" max="23" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="21"/>
+    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27"/>
+      <c r="M14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="33"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="I15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="K15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="21">
+        <v>5</v>
+      </c>
+      <c r="O15" s="21">
+        <v>5</v>
+      </c>
+      <c r="P15" s="21">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>5</v>
+      </c>
+      <c r="R15" s="21">
+        <v>5</v>
+      </c>
+      <c r="S15" s="21">
+        <v>5</v>
+      </c>
+      <c r="T15" s="21">
+        <v>5</v>
+      </c>
+      <c r="U15" s="22">
+        <v>5</v>
+      </c>
+      <c r="V15" s="23"/>
+      <c r="W15" s="24"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C16" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D16" s="4">
         <v>1.5</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E16" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F16" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G16" s="4">
         <v>1.7</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H16" s="4">
         <v>5</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I16" s="4">
         <f>PRODUCT(Tabel2[[#This Row],[do]:[as]])</f>
         <v>1.5</v>
       </c>
-      <c r="J3" s="14">
-        <f>MROUND(PRODUCT(B3,E3,I3), 1) + F3 + G3</f>
+      <c r="J16" s="10">
+        <f>MROUND(PRODUCT(B16,E16,I16), 1) + F16 + G16</f>
         <v>4.7</v>
       </c>
-      <c r="K3" s="13">
-        <f t="shared" ref="K3:K7" si="0">H3/J3</f>
+      <c r="K16" s="9">
+        <f>H16/J16</f>
         <v>1.0638297872340425</v>
       </c>
+      <c r="M16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B17" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E17" s="4">
         <v>1.5</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F17" s="4">
         <v>3</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G17" s="4">
         <v>8</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H17" s="4">
         <v>15</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I17" s="4">
         <f>PRODUCT(Tabel2[[#This Row],[do]:[as]])</f>
         <v>1</v>
       </c>
-      <c r="J4" s="12">
-        <f t="shared" ref="J4:J7" si="1">MROUND(PRODUCT(B4,E4,I4), 1) + F4 + G4</f>
+      <c r="J17" s="8">
+        <f>MROUND(PRODUCT(B17,E17,I17), 1) + F17 + G17</f>
         <v>13</v>
       </c>
-      <c r="K4" s="13">
-        <f t="shared" si="0"/>
+      <c r="K17" s="9">
+        <f>H17/J17</f>
         <v>1.1538461538461537</v>
       </c>
+      <c r="M17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" s="4">
+        <f>PRODUCT(N15,B16)</f>
+        <v>10</v>
+      </c>
+      <c r="O17" s="4">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>1</v>
+      </c>
+      <c r="R17" s="4">
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="T17" s="4">
+        <v>5</v>
+      </c>
+      <c r="U17" s="4">
+        <f>PRODUCT(Tabel24[[#This Row],[do]:[as]])</f>
+        <v>1.5</v>
+      </c>
+      <c r="V17" s="10">
+        <f>MROUND(PRODUCT(N17,Q17,U17), 1) + R17 + S17</f>
+        <v>16.7</v>
+      </c>
+      <c r="W17" s="9">
+        <f t="shared" ref="W17:W21" si="0">T17/V17</f>
+        <v>0.29940119760479045</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="6">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C18" s="4">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D18" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E18" s="4">
         <v>0.5</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F18" s="4">
         <v>3</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G18" s="4">
         <v>8</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H18" s="4">
         <v>20</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I18" s="4">
         <f>PRODUCT(Tabel2[[#This Row],[do]:[as]])</f>
         <v>2</v>
       </c>
-      <c r="J5" s="12">
-        <f>MROUND(PRODUCT(B5,E5,I5), 1) + F5 + G5</f>
+      <c r="J18" s="8">
+        <f>MROUND(PRODUCT(B18,E18,I18), 1) + F18 + G18</f>
         <v>14</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K18" s="9">
+        <f>H18/J18</f>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="4">
+        <f>PRODUCT(N15,B17)</f>
+        <v>5</v>
+      </c>
+      <c r="O18" s="4">
+        <v>1</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="R18" s="4">
+        <v>3</v>
+      </c>
+      <c r="S18" s="4">
+        <v>8</v>
+      </c>
+      <c r="T18" s="4">
+        <v>15</v>
+      </c>
+      <c r="U18" s="4">
+        <f>PRODUCT(Tabel24[[#This Row],[do]:[as]])</f>
+        <v>1</v>
+      </c>
+      <c r="V18" s="8">
+        <f t="shared" ref="V18" si="1">MROUND(PRODUCT(N18,Q18,U18), 1) + R18 + S18</f>
+        <v>19</v>
+      </c>
+      <c r="W18" s="9">
         <f t="shared" si="0"/>
-        <v>1.4285714285714286</v>
+        <v>0.78947368421052633</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B19" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C19" s="4">
         <v>15</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D19" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E19" s="4">
         <v>0.5</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F19" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G19" s="4">
         <v>1.7</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H19" s="4">
         <v>80</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I19" s="4">
         <f>PRODUCT(Tabel2[[#This Row],[do]:[as]])</f>
         <v>15</v>
       </c>
-      <c r="J6" s="12">
-        <f t="shared" si="1"/>
+      <c r="J19" s="8">
+        <f>MROUND(PRODUCT(B19,E19,I19), 1) + F19 + G19</f>
         <v>39.700000000000003</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K19" s="9">
+        <f>H19/J19</f>
+        <v>2.0151133501259446</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="4">
+        <f>PRODUCT(N15,B18)</f>
+        <v>15</v>
+      </c>
+      <c r="O19" s="4">
+        <v>2</v>
+      </c>
+      <c r="P19" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="R19" s="4">
+        <v>3</v>
+      </c>
+      <c r="S19" s="4">
+        <v>8</v>
+      </c>
+      <c r="T19" s="4">
+        <v>20</v>
+      </c>
+      <c r="U19" s="4">
+        <f>PRODUCT(Tabel24[[#This Row],[do]:[as]])</f>
+        <v>2</v>
+      </c>
+      <c r="V19" s="8">
+        <f>MROUND(PRODUCT(N19,Q19,U19), 1) + R19 + S19</f>
+        <v>26</v>
+      </c>
+      <c r="W19" s="9">
         <f t="shared" si="0"/>
-        <v>2.0151133501259446</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B20" s="4">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C20" s="4">
         <v>15</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D20" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E20" s="4">
         <v>0.5</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F20" s="4">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G20" s="4">
         <v>1.7</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H20" s="4">
         <v>160</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I20" s="4">
         <f>PRODUCT(Tabel2[[#This Row],[do]:[as]])</f>
         <v>15</v>
       </c>
-      <c r="J7" s="12">
-        <f t="shared" si="1"/>
+      <c r="J20" s="8">
+        <f>MROUND(PRODUCT(B20,E20,I20), 1) + F20 + G20</f>
         <v>76.7</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K20" s="9">
+        <f>H20/J20</f>
+        <v>2.0860495436766624</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" s="4">
+        <f>PRODUCT(N15,B19)</f>
+        <v>25</v>
+      </c>
+      <c r="O20" s="4">
+        <v>15</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0</v>
+      </c>
+      <c r="S20" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="T20" s="4">
+        <v>80</v>
+      </c>
+      <c r="U20" s="4">
+        <f>PRODUCT(Tabel24[[#This Row],[do]:[as]])</f>
+        <v>15</v>
+      </c>
+      <c r="V20" s="8">
+        <f t="shared" ref="V20:V21" si="2">MROUND(PRODUCT(N20,Q20,U20), 1) + R20 + S20</f>
+        <v>189.7</v>
+      </c>
+      <c r="W20" s="9">
         <f t="shared" si="0"/>
-        <v>2.0860495436766624</v>
+        <v>0.42171850289931473</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="s">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="14">
+        <f>PRODUCT(N15,B20)</f>
+        <v>50</v>
+      </c>
+      <c r="O21" s="14">
+        <v>15</v>
+      </c>
+      <c r="P21" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="R21" s="14">
+        <v>0</v>
+      </c>
+      <c r="S21" s="14">
+        <v>1.7</v>
+      </c>
+      <c r="T21" s="14">
+        <v>160</v>
+      </c>
+      <c r="U21" s="14">
+        <f>PRODUCT(Tabel24[[#This Row],[do]:[as]])</f>
+        <v>15</v>
+      </c>
+      <c r="V21" s="16">
+        <f t="shared" si="2"/>
+        <v>376.7</v>
+      </c>
+      <c r="W21" s="19">
+        <f t="shared" si="0"/>
+        <v>0.4247411733474914</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M22" s="18"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="17"/>
+    </row>
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="30"/>
+      <c r="M27" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="30"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="10" t="s">
+    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D28" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>28</v>
+      <c r="E28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="N28" s="11">
+        <v>5</v>
+      </c>
+      <c r="O28" s="11">
+        <v>5</v>
+      </c>
+      <c r="P28" s="11">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="11">
+        <v>5</v>
+      </c>
+      <c r="R28" s="13">
+        <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1">
         <v>100</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C29" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D29" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E29" s="1">
         <v>5</v>
       </c>
-      <c r="F16" s="1">
-        <f t="shared" ref="F16:F17" si="2">PRODUCT(C16,D16)</f>
+      <c r="F29" s="1">
+        <f t="shared" ref="F29:F30" si="3">PRODUCT(C29,D29)</f>
         <v>1</v>
       </c>
+      <c r="M29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
-        <f t="shared" si="2"/>
+      <c r="N30" s="1">
+        <v>100</v>
+      </c>
+      <c r="O30" s="1">
+        <v>1</v>
+      </c>
+      <c r="P30" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>5</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" ref="R30:R31" si="4">PRODUCT(O30,P30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M31" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A14:F14"/>
+  <mergeCells count="4">
+    <mergeCell ref="A14:K14"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="M14:W14"/>
+    <mergeCell ref="M27:R27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>